<commit_message>
Fix missing of checking for. Add better documentation
</commit_message>
<xml_diff>
--- a/evaluation-vuze/csvs/random100/evaluation.xlsx
+++ b/evaluation-vuze/csvs/random100/evaluation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13900" yWindow="2980" windowWidth="25600" windowHeight="19940" tabRatio="500"/>
+    <workbookView xWindow="51200" yWindow="4320" windowWidth="25600" windowHeight="19940" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="eval_top5package" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="172">
   <si>
     <t>package</t>
   </si>
@@ -474,13 +474,73 @@
     <t>/top5package/org/json/simple/JSONValue.java</t>
   </si>
   <si>
+    <t>The three missing are not possible to be detected by our heuristics because all of the types are int. Manually notation is needed</t>
+  </si>
+  <si>
     <t>Comments</t>
   </si>
   <si>
+    <t>The three missing are due to the missing knowledge about method call that are time related</t>
+  </si>
+  <si>
     <t>DataOutputStream dos = new DataOutputStream( socket.getOutputStream())</t>
   </si>
   <si>
     <t>SocketTimeout</t>
+  </si>
+  <si>
+    <t>Create an issue for this</t>
+  </si>
+  <si>
+    <t>accept_idle &gt; 10 * 60 * 1000</t>
+  </si>
+  <si>
+    <t>last_non_local_connection_time &gt; SystemTime.getCurrentTime()</t>
+  </si>
+  <si>
+    <t>now - last_modified &gt; 10 * 24 * 60 * 60 * 1000L</t>
+  </si>
+  <si>
+    <t>last_mod &gt; most_recent_time &amp;&amp; last_mod &gt; one_week_ago</t>
+  </si>
+  <si>
+    <t>now &lt; last_write_select_debug ||       now - last_write_select_debug &gt; WRITE_SELECTOR_DEBUG_CHECK_PERIOD</t>
+  </si>
+  <si>
+    <t>stall_time &lt; 0</t>
+  </si>
+  <si>
+    <t>stall_time &gt; WRITE_SELECTOR_DEBUG_MAX_TIME</t>
+  </si>
+  <si>
+    <t>time_diff &lt; timeout &amp;&amp; time_diff &gt;= 0</t>
+  </si>
+  <si>
+    <t>end &gt; start</t>
+  </si>
+  <si>
+    <t>elapsed &gt; ( (long)WARN_TIME * (x.warn_count+1))</t>
+  </si>
+  <si>
+    <t>execution_limit &gt; 0 &amp;&amp; elapsed &gt; execution_limit</t>
+  </si>
+  <si>
+    <t>org.gudy.azureus2.core3.util.ThreadPool</t>
+  </si>
+  <si>
+    <t>SystemTime.getCurrentTime() - start_time &gt; 30*1000</t>
+  </si>
+  <si>
+    <t>SystemTime.getCurrentTime() - read_start_time &gt; 30*1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The missing is for a method call that return time type. </t>
+  </si>
+  <si>
+    <t>The missing is fault of we just check if it is a direct call to a method, not if in the expr there is a method with such name :/</t>
+  </si>
+  <si>
+    <t>Must set manually that is a timer object, line 147.</t>
   </si>
 </sst>
 </file>
@@ -516,13 +576,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -535,7 +610,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F1048576" totalsRowShown="0">
   <autoFilter ref="A1:F1048576"/>
-  <sortState ref="A2:F97">
+  <sortState ref="A2:F56">
     <sortCondition ref="B1:B1048576"/>
   </sortState>
   <tableColumns count="6">
@@ -544,7 +619,7 @@
     <tableColumn id="3" name="line"/>
     <tableColumn id="4" name="code"/>
     <tableColumn id="5" name="type"/>
-    <tableColumn id="6" name="correct"/>
+    <tableColumn id="6" name="correct" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -831,21 +906,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:L42"/>
+    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="91.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="91.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="93.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -861,11 +938,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -881,87 +958,51 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2">
-        <v>504</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3">
+        <v>235</v>
+      </c>
+      <c r="D3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>365</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3">
-        <v>146</v>
-      </c>
-      <c r="K3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>146</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4">
-        <v>158</v>
-      </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -969,31 +1010,19 @@
         <v>16</v>
       </c>
       <c r="C5">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5">
-        <v>254</v>
-      </c>
-      <c r="K5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1001,31 +1030,19 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <v>254</v>
+        <v>158</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6">
-        <v>266</v>
-      </c>
-      <c r="K6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1033,31 +1050,19 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="H7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7">
-        <v>472</v>
-      </c>
-      <c r="K7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1065,319 +1070,199 @@
         <v>16</v>
       </c>
       <c r="C8">
-        <v>472</v>
+        <v>266</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="H8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J8">
-        <v>598</v>
-      </c>
-      <c r="K8" t="s">
-        <v>49</v>
-      </c>
-      <c r="L8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>504</v>
+        <v>472</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="H9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J9">
-        <v>238</v>
-      </c>
-      <c r="K9" t="s">
-        <v>51</v>
-      </c>
-      <c r="L9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>339</v>
+        <v>504</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="H10" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J10">
-        <v>130</v>
-      </c>
-      <c r="K10" t="s">
-        <v>52</v>
-      </c>
-      <c r="L10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11">
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>155</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" t="s">
-        <v>50</v>
-      </c>
-      <c r="I11" t="s">
-        <v>48</v>
-      </c>
-      <c r="J11">
-        <v>394</v>
-      </c>
-      <c r="K11" t="s">
-        <v>51</v>
-      </c>
-      <c r="L11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C12">
-        <v>142</v>
+        <v>389</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12">
-        <v>610</v>
-      </c>
-      <c r="K12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C13">
-        <v>323</v>
+        <v>339</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
-      <c r="H13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13">
-        <v>917</v>
-      </c>
-      <c r="K13" t="s">
-        <v>7</v>
-      </c>
-      <c r="L13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C14">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>167</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" t="s">
-        <v>28</v>
-      </c>
-      <c r="J14">
-        <v>323</v>
-      </c>
-      <c r="K14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C15">
-        <v>330</v>
+        <v>357</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>168</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" t="s">
-        <v>28</v>
-      </c>
-      <c r="J15">
-        <v>328</v>
-      </c>
-      <c r="K15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C16">
-        <v>353</v>
+        <v>130</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
-      <c r="H16" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J16">
-        <v>330</v>
-      </c>
-      <c r="K16" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17">
-        <v>381</v>
+        <v>142</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
       </c>
-      <c r="H17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17">
-        <v>353</v>
-      </c>
-      <c r="K17" t="s">
-        <v>30</v>
-      </c>
-      <c r="L17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1385,31 +1270,19 @@
         <v>28</v>
       </c>
       <c r="C18">
-        <v>591</v>
+        <v>323</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
       </c>
-      <c r="H18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" t="s">
-        <v>28</v>
-      </c>
-      <c r="J18">
-        <v>381</v>
-      </c>
-      <c r="K18" t="s">
-        <v>30</v>
-      </c>
-      <c r="L18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1417,31 +1290,19 @@
         <v>28</v>
       </c>
       <c r="C19">
-        <v>598</v>
+        <v>328</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="H19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I19" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19">
-        <v>591</v>
-      </c>
-      <c r="K19" t="s">
-        <v>30</v>
-      </c>
-      <c r="L19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1449,7 +1310,7 @@
         <v>28</v>
       </c>
       <c r="C20">
-        <v>745</v>
+        <v>330</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1457,23 +1318,11 @@
       <c r="E20" t="s">
         <v>8</v>
       </c>
-      <c r="H20" t="s">
-        <v>20</v>
-      </c>
-      <c r="I20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20">
-        <v>598</v>
-      </c>
-      <c r="K20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1481,31 +1330,19 @@
         <v>28</v>
       </c>
       <c r="C21">
-        <v>763</v>
+        <v>353</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
       </c>
-      <c r="H21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I21" t="s">
-        <v>28</v>
-      </c>
-      <c r="J21">
-        <v>745</v>
-      </c>
-      <c r="K21" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1513,31 +1350,19 @@
         <v>28</v>
       </c>
       <c r="C22">
-        <v>1115</v>
+        <v>381</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
       </c>
-      <c r="H22" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" t="s">
-        <v>28</v>
-      </c>
-      <c r="J22">
-        <v>763</v>
-      </c>
-      <c r="K22" t="s">
-        <v>31</v>
-      </c>
-      <c r="L22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1545,31 +1370,19 @@
         <v>28</v>
       </c>
       <c r="C23">
-        <v>585</v>
+        <v>591</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" t="s">
-        <v>20</v>
-      </c>
-      <c r="I23" t="s">
-        <v>28</v>
-      </c>
-      <c r="J23">
-        <v>1115</v>
-      </c>
-      <c r="K23" t="s">
-        <v>32</v>
-      </c>
-      <c r="L23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1577,31 +1390,19 @@
         <v>28</v>
       </c>
       <c r="C24">
-        <v>737</v>
+        <v>598</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" t="s">
-        <v>20</v>
-      </c>
-      <c r="I24" t="s">
-        <v>28</v>
-      </c>
-      <c r="J24">
-        <v>585</v>
-      </c>
-      <c r="K24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1609,557 +1410,570 @@
         <v>28</v>
       </c>
       <c r="C25">
-        <v>752</v>
+        <v>745</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26">
+        <v>763</v>
+      </c>
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>1115</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28">
+        <v>585</v>
+      </c>
+      <c r="D28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" t="s">
         <v>9</v>
       </c>
-      <c r="H25" t="s">
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>20</v>
       </c>
-      <c r="I25" t="s">
+      <c r="B29" t="s">
         <v>28</v>
       </c>
-      <c r="J25">
+      <c r="C29">
         <v>737</v>
       </c>
-      <c r="K25" t="s">
+      <c r="D29" t="s">
         <v>34</v>
-      </c>
-      <c r="L25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26">
-        <v>1099</v>
-      </c>
-      <c r="D26" t="s">
-        <v>38</v>
-      </c>
-      <c r="E26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" t="s">
-        <v>28</v>
-      </c>
-      <c r="J26">
-        <v>752</v>
-      </c>
-      <c r="K26" t="s">
-        <v>35</v>
-      </c>
-      <c r="L26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27">
-        <v>1295</v>
-      </c>
-      <c r="D27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" t="s">
-        <v>42</v>
-      </c>
-      <c r="I27" t="s">
-        <v>43</v>
-      </c>
-      <c r="J27">
-        <v>78</v>
-      </c>
-      <c r="K27" t="s">
-        <v>44</v>
-      </c>
-      <c r="L27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28">
-        <v>2023</v>
-      </c>
-      <c r="D28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" t="s">
-        <v>6</v>
-      </c>
-      <c r="I28" t="s">
-        <v>10</v>
-      </c>
-      <c r="J28">
-        <v>359</v>
-      </c>
-      <c r="K28" t="s">
-        <v>11</v>
-      </c>
-      <c r="L28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29">
-        <v>2014</v>
-      </c>
-      <c r="D29" t="s">
-        <v>41</v>
       </c>
       <c r="E29" t="s">
         <v>9</v>
       </c>
-      <c r="H29" t="s">
-        <v>6</v>
-      </c>
-      <c r="I29" t="s">
-        <v>115</v>
-      </c>
-      <c r="J29">
-        <v>235</v>
-      </c>
-      <c r="K29" t="s">
-        <v>150</v>
-      </c>
-      <c r="L29" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C30">
-        <v>78</v>
+        <v>752</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" t="s">
-        <v>36</v>
-      </c>
-      <c r="I30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J30">
-        <v>1099</v>
-      </c>
-      <c r="K30" t="s">
-        <v>38</v>
-      </c>
-      <c r="L30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C31">
-        <v>610</v>
+        <v>848</v>
       </c>
       <c r="D31" t="s">
-        <v>19</v>
+        <v>159</v>
       </c>
       <c r="E31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I31" t="s">
-        <v>37</v>
-      </c>
-      <c r="J31">
-        <v>1295</v>
-      </c>
-      <c r="K31" t="s">
-        <v>39</v>
-      </c>
-      <c r="L31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C32">
-        <v>917</v>
+        <v>1071</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>160</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" t="s">
-        <v>40</v>
-      </c>
-      <c r="I32" t="s">
-        <v>37</v>
-      </c>
-      <c r="J32">
-        <v>2023</v>
-      </c>
-      <c r="K32" t="s">
-        <v>15</v>
-      </c>
-      <c r="L32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C33">
-        <v>104</v>
+        <v>1077</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>161</v>
       </c>
       <c r="E33" t="s">
         <v>9</v>
       </c>
-      <c r="H33" t="s">
-        <v>40</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34">
+        <v>1114</v>
+      </c>
+      <c r="D34" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
         <v>37</v>
       </c>
-      <c r="J33">
-        <v>2014</v>
-      </c>
-      <c r="K33" t="s">
-        <v>41</v>
-      </c>
-      <c r="L33" t="s">
+      <c r="C35">
+        <v>1099</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34">
-        <v>598</v>
-      </c>
-      <c r="D34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34" t="s">
-        <v>42</v>
-      </c>
-      <c r="I34" t="s">
-        <v>55</v>
-      </c>
-      <c r="J34">
-        <v>4638</v>
-      </c>
-      <c r="K34" t="s">
-        <v>56</v>
-      </c>
-      <c r="L34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35">
-        <v>238</v>
-      </c>
-      <c r="D35" t="s">
-        <v>51</v>
-      </c>
-      <c r="E35" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" t="s">
-        <v>42</v>
-      </c>
-      <c r="I35" t="s">
-        <v>55</v>
-      </c>
-      <c r="J35">
-        <v>3853</v>
-      </c>
-      <c r="K35" t="s">
-        <v>57</v>
-      </c>
-      <c r="L35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C36">
-        <v>130</v>
+        <v>1295</v>
       </c>
       <c r="D36" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E36" t="s">
         <v>9</v>
       </c>
-      <c r="H36" t="s">
-        <v>42</v>
-      </c>
-      <c r="I36" t="s">
-        <v>55</v>
-      </c>
-      <c r="J36">
-        <v>3895</v>
-      </c>
-      <c r="K36" t="s">
-        <v>58</v>
-      </c>
-      <c r="L36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C37">
-        <v>394</v>
+        <v>2023</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="E37" t="s">
         <v>8</v>
       </c>
-      <c r="H37" t="s">
-        <v>42</v>
-      </c>
-      <c r="I37" t="s">
-        <v>53</v>
-      </c>
-      <c r="J37">
-        <v>579</v>
-      </c>
-      <c r="K37" t="s">
-        <v>54</v>
-      </c>
-      <c r="L37" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C38">
-        <v>579</v>
+        <v>2014</v>
       </c>
       <c r="D38" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E38" t="s">
         <v>9</v>
       </c>
-      <c r="H38" t="s">
-        <v>20</v>
-      </c>
-      <c r="I38" t="s">
-        <v>25</v>
-      </c>
-      <c r="J38">
-        <v>130</v>
-      </c>
-      <c r="K38" t="s">
-        <v>26</v>
-      </c>
-      <c r="L38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="C39">
-        <v>4638</v>
+        <v>288</v>
       </c>
       <c r="D39" t="s">
-        <v>56</v>
+        <v>157</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
-      </c>
-      <c r="H39" t="s">
-        <v>20</v>
-      </c>
-      <c r="I39" t="s">
-        <v>27</v>
-      </c>
-      <c r="J39">
-        <v>142</v>
-      </c>
-      <c r="K39" t="s">
-        <v>15</v>
-      </c>
-      <c r="L39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="C40">
-        <v>3853</v>
+        <v>507</v>
       </c>
       <c r="D40" t="s">
-        <v>57</v>
+        <v>158</v>
       </c>
       <c r="E40" t="s">
         <v>9</v>
       </c>
-      <c r="H40" t="s">
-        <v>13</v>
-      </c>
-      <c r="I40" t="s">
-        <v>14</v>
-      </c>
-      <c r="J40">
-        <v>365</v>
-      </c>
-      <c r="K40" t="s">
-        <v>15</v>
-      </c>
-      <c r="L40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
       <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41">
+        <v>78</v>
+      </c>
+      <c r="D41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42">
+        <v>610</v>
+      </c>
+      <c r="D42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43">
+        <v>917</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44">
+        <v>104</v>
+      </c>
+      <c r="D44" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45">
+        <v>641</v>
+      </c>
+      <c r="D45" t="s">
+        <v>163</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46">
+        <v>598</v>
+      </c>
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47">
+        <v>238</v>
+      </c>
+      <c r="D47" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48">
+        <v>130</v>
+      </c>
+      <c r="D48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>394</v>
+      </c>
+      <c r="D49" t="s">
+        <v>51</v>
+      </c>
+      <c r="E49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50">
+        <v>527</v>
+      </c>
+      <c r="D50" t="s">
+        <v>164</v>
+      </c>
+      <c r="E50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51">
+        <v>536</v>
+      </c>
+      <c r="D51" t="s">
+        <v>165</v>
+      </c>
+      <c r="E51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52">
+        <v>579</v>
+      </c>
+      <c r="D52" t="s">
+        <v>54</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>166</v>
+      </c>
+      <c r="B53" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53">
+        <v>745</v>
+      </c>
+      <c r="D53" t="s">
+        <v>54</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" t="s">
         <v>55</v>
       </c>
-      <c r="C41">
+      <c r="C54">
+        <v>4638</v>
+      </c>
+      <c r="D54" t="s">
+        <v>56</v>
+      </c>
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55">
+        <v>3853</v>
+      </c>
+      <c r="D55" t="s">
+        <v>57</v>
+      </c>
+      <c r="E55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56">
         <v>3895</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D56" t="s">
         <v>58</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E56" t="s">
         <v>9</v>
-      </c>
-      <c r="H41" t="s">
-        <v>42</v>
-      </c>
-      <c r="I41" t="s">
-        <v>46</v>
-      </c>
-      <c r="J41">
-        <v>104</v>
-      </c>
-      <c r="K41" t="s">
-        <v>47</v>
-      </c>
-      <c r="L41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H42" t="s">
-        <v>20</v>
-      </c>
-      <c r="I42" t="s">
-        <v>23</v>
-      </c>
-      <c r="J42">
-        <v>339</v>
-      </c>
-      <c r="K42" t="s">
-        <v>24</v>
-      </c>
-      <c r="L42" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2174,8 +1988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F6"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2183,6 +1997,7 @@
     <col min="1" max="1" width="146.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="104.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -2202,160 +2017,418 @@
         <v>63</v>
       </c>
       <c r="F1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>85</v>
       </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>111</v>
       </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>127</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>115</v>
       </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>131</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>125</v>
       </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>133</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>135</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>67</v>
       </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
add result of evaluation
</commit_message>
<xml_diff>
--- a/evaluation-vuze/csvs/random100/evaluation.xlsx
+++ b/evaluation-vuze/csvs/random100/evaluation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="4320" windowWidth="25600" windowHeight="19940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-28800" yWindow="11260" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="eval_top5package" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="187">
   <si>
     <t>package</t>
   </si>
@@ -541,12 +541,60 @@
   </si>
   <si>
     <t>Must set manually that is a timer object, line 147.</t>
+  </si>
+  <si>
+    <t>3xSimpleTimer class event not recognise because user should set it as time type. Missing % operator. DelayedEvent must set as tyme type by user. Socket.connect can have timeout. Parameter of class as long must manually set as time. 2x No HttpURLConnection support.</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F-Measure</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>SimpleTimer must manually set as time. We miss because we do not check if we assign a var time to another var</t>
+  </si>
+  <si>
+    <t>Timer must defined by the user.</t>
+  </si>
+  <si>
+    <t>int vars must be expressed manually as time.</t>
+  </si>
+  <si>
+    <t>SimpleTime must be defined manually as time.</t>
+  </si>
+  <si>
+    <t>SimpleTime must be defined manually as time. Timer must be defined manually as time.</t>
+  </si>
+  <si>
+    <t>DelayedEvent must be defined manually as time.</t>
+  </si>
+  <si>
+    <t>int vars must be expressed manually as time. Method getTime must manually defined or double parse</t>
+  </si>
+  <si>
+    <t>int vars must be expressed manually as time. SimplerTime must be defined manually as time.</t>
+  </si>
+  <si>
+    <t>there are some checks of the time, but they are for format a string and therefore not relevant.</t>
+  </si>
+  <si>
+    <t>SimpleTime must be defined manually as time. Int vars must be expressed manually as time.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -576,14 +624,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -619,7 +672,7 @@
     <tableColumn id="3" name="line"/>
     <tableColumn id="4" name="code"/>
     <tableColumn id="5" name="type"/>
-    <tableColumn id="6" name="correct" dataDxfId="0"/>
+    <tableColumn id="6" name="correct" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -633,7 +686,7 @@
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="How Many"/>
+    <tableColumn id="2" name="How Many" dataDxfId="0"/>
     <tableColumn id="3" name="Correct"/>
     <tableColumn id="4" name="Incorrect"/>
     <tableColumn id="5" name="Missing"/>
@@ -908,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView showRuler="0" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1986,16 +2039,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B72" workbookViewId="0">
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="146.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="93" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" customWidth="1"/>
     <col min="6" max="6" width="104.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2004,7 +2057,7 @@
       <c r="A1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C1" t="s">
@@ -2024,7 +2077,7 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>4</v>
       </c>
       <c r="C2">
@@ -2044,7 +2097,7 @@
       <c r="A3" t="s">
         <v>85</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0</v>
       </c>
       <c r="C3">
@@ -2061,7 +2114,7 @@
       <c r="A4" t="s">
         <v>111</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4">
@@ -2081,7 +2134,7 @@
       <c r="A5" t="s">
         <v>127</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>0</v>
       </c>
       <c r="C5">
@@ -2098,7 +2151,7 @@
       <c r="A6" t="s">
         <v>115</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6">
@@ -2118,7 +2171,7 @@
       <c r="A7" t="s">
         <v>131</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>0</v>
       </c>
       <c r="C7">
@@ -2135,7 +2188,7 @@
       <c r="A8" t="s">
         <v>125</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>2</v>
       </c>
       <c r="C8">
@@ -2155,7 +2208,7 @@
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>1</v>
       </c>
       <c r="C9">
@@ -2172,7 +2225,7 @@
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>5</v>
       </c>
       <c r="C10">
@@ -2189,7 +2242,7 @@
       <c r="A11" t="s">
         <v>133</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>0</v>
       </c>
       <c r="C11">
@@ -2206,7 +2259,7 @@
       <c r="A12" t="s">
         <v>135</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>0</v>
       </c>
       <c r="C12">
@@ -2223,7 +2276,7 @@
       <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>3</v>
       </c>
       <c r="C13">
@@ -2240,7 +2293,7 @@
       <c r="A14" t="s">
         <v>67</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>0</v>
       </c>
       <c r="C14">
@@ -2257,7 +2310,7 @@
       <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>3</v>
       </c>
       <c r="C15">
@@ -2274,7 +2327,7 @@
       <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>0</v>
       </c>
       <c r="C16">
@@ -2294,7 +2347,7 @@
       <c r="A17" t="s">
         <v>95</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>0</v>
       </c>
       <c r="C17">
@@ -2311,7 +2364,7 @@
       <c r="A18" t="s">
         <v>126</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>0</v>
       </c>
       <c r="C18">
@@ -2328,7 +2381,7 @@
       <c r="A19" t="s">
         <v>70</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>0</v>
       </c>
       <c r="C19">
@@ -2345,7 +2398,7 @@
       <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <v>0</v>
       </c>
       <c r="C20">
@@ -2362,7 +2415,7 @@
       <c r="A21" t="s">
         <v>28</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="3">
         <v>18</v>
       </c>
       <c r="C21">
@@ -2382,400 +2435,1459 @@
       <c r="A22" t="s">
         <v>37</v>
       </c>
+      <c r="B22" s="3">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>143</v>
       </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>87</v>
       </c>
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>64</v>
       </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>102</v>
       </c>
+      <c r="B26" s="3">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>140</v>
       </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>147</v>
       </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>123</v>
       </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>128</v>
       </c>
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>43</v>
       </c>
+      <c r="B31" s="3">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" s="3">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" s="3">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" s="3">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" s="3">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" s="3">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39" s="3">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40" s="3">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B42" s="3">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B43" s="3">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B44" s="3">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B45" s="3">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B46" s="3">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B47" s="3">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48" s="3">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49" s="3">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B50" s="3">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B51" s="3">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B52" s="3">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B53" s="3">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B54" s="3">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B55" s="3">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B56" s="3">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B57" s="3">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B58" s="3">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B59" s="3">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B60" s="3">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B61" s="3">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B62" s="3">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B63" s="3">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B64" s="3">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B65" s="3">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B66" s="3">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B67" s="3">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B68" s="3">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B69" s="3">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B70" s="3">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B71" s="3">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B72" s="3">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B73" s="3">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B74" s="3">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B75" s="3">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B76" s="3">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B77" s="3">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B78" s="3">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B79" s="3">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B80" s="3">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B81" s="3">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B82" s="3">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B83" s="3">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B84" s="3">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B85" s="3">
+        <v>6</v>
+      </c>
+      <c r="C85">
+        <v>4</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="F85" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B86" s="3">
+        <v>6</v>
+      </c>
+      <c r="C86">
+        <v>4</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>2</v>
+      </c>
+      <c r="F86" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B87" s="3">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B88" s="3">
+        <v>2</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="F88" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B89" s="3">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B90" s="3">
+        <v>2</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>2</v>
+      </c>
+      <c r="F90" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B91" s="3">
+        <v>8</v>
+      </c>
+      <c r="C91">
+        <v>3</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>5</v>
+      </c>
+      <c r="F91" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B92" s="3">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B93" s="3">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B94" s="3">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B95" s="3">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B96" s="3">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B97" s="3">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B98" s="3">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B99" s="3">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B100" s="3">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>120</v>
+      </c>
+      <c r="B101" s="3">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B104" s="3">
+        <f>SUM(B1:B101)</f>
+        <v>95</v>
+      </c>
+      <c r="C104">
+        <f t="shared" ref="C104:E104" si="0">SUM(C1:C101)</f>
+        <v>55</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>174</v>
+      </c>
+      <c r="B106" s="2">
+        <f>C104/B104*100</f>
+        <v>57.894736842105267</v>
+      </c>
+      <c r="C106" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>173</v>
+      </c>
+      <c r="B107" s="2">
+        <f>(C104-D104)/C104*100</f>
+        <v>100</v>
+      </c>
+      <c r="C107" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>175</v>
+      </c>
+      <c r="B108" s="2">
+        <f>2*(B107*B106)/(B107+B106)</f>
+        <v>73.333333333333343</v>
+      </c>
+      <c r="C108" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First commit on indexing branch
</commit_message>
<xml_diff>
--- a/evaluation-vuze/csvs/random100/evaluation.xlsx
+++ b/evaluation-vuze/csvs/random100/evaluation.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="11260" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="11200" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="eval_top5package" sheetId="1" r:id="rId1"/>
     <sheet name="List of file" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2041,8 +2041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B72" workbookViewId="0">
-      <selection activeCell="F101" sqref="F101"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>